<commit_message>
predefined list into participants template
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>Identification number</t>
   </si>
 </sst>
 </file>
@@ -112,10 +112,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -166,16 +169,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1009650</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4324350</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -198,7 +201,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3028950" y="171450"/>
+          <a:off x="6105525" y="133350"/>
           <a:ext cx="3343275" cy="1371600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -474,18 +477,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="80.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1" collapsed="1"/>
@@ -494,71 +499,165 @@
     <col min="15" max="15" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <mergeCells count="11">
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D1048576">
       <formula1>"F,M"</formula1>
     </dataValidation>
   </dataValidations>
@@ -575,6 +674,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.140625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -587,6 +689,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="105.140625" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
data validator highest degree and funding type for participants template
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -13,8 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="participants" sheetId="1" r:id="rId1"/>
-    <sheet name="countries" sheetId="2" r:id="rId2"/>
-    <sheet name="institutions" sheetId="3" r:id="rId3"/>
+    <sheet name="funding_type" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="highest_degree" sheetId="5" state="hidden" r:id="rId3"/>
+    <sheet name="countries" sheetId="2" state="hidden" r:id="rId4"/>
+    <sheet name="institutions" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="countriesList">#REF!</definedName>
@@ -480,7 +482,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,6 +676,32 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
   </cols>
@@ -682,7 +710,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
field other for gender in html form and template.
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Funding Type</t>
+  </si>
+  <si>
+    <t>Suggest Intitution</t>
   </si>
 </sst>
 </file>
@@ -211,6 +214,91 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14430375" y="0"/>
+          <a:ext cx="2676525" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFCC"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>If you don't find the institution you are looking for, suggest it by typing in the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1400" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> suggest institution </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>column.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -479,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection sqref="A1:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,12 +584,13 @@
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.140625" customWidth="1"/>
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
     <col min="15" max="15" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -513,8 +602,9 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -526,8 +616,9 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -539,8 +630,9 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -552,8 +644,9 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -565,8 +658,9 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -578,8 +672,9 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -591,8 +686,9 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -604,8 +700,9 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -617,8 +714,9 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -651,12 +749,15 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:K9"/>
+    <mergeCell ref="A1:L9"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10 D12:D1048576">

</xml_diff>

<commit_message>
change gender data validator
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -570,7 +570,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,12 +759,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:L9"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10 D12:D1048576">
-      <formula1>"F,M"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11">
-      <formula1>"F,M,Other"</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"Male, Famale, Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
capdev summaries by research program
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Identification number</t>
-  </si>
-  <si>
-    <t>Funding Type</t>
   </si>
   <si>
     <t>Suggest Intitution</t>
@@ -218,14 +215,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1390651</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -236,8 +233,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14430375" y="0"/>
-          <a:ext cx="2676525" cy="971550"/>
+          <a:off x="13496925" y="0"/>
+          <a:ext cx="2428876" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -567,10 +564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,14 +580,13 @@
     <col min="7" max="7" width="80.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -602,9 +598,8 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -616,9 +611,8 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -630,9 +624,8 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -644,9 +637,8 @@
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -658,9 +650,8 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -672,9 +663,8 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -686,9 +676,8 @@
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -700,9 +689,8 @@
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -714,9 +702,8 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -749,15 +736,12 @@
       </c>
       <c r="K10" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:L9"/>
+    <mergeCell ref="A1:K9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">

</xml_diff>

<commit_message>
create detail sheet into capdev summary
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Country of institution</t>
-  </si>
-  <si>
-    <t>Reference</t>
   </si>
   <si>
     <t>Email</t>
@@ -215,13 +212,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>1390651</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -233,8 +230,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13496925" y="0"/>
-          <a:ext cx="2428876" cy="971550"/>
+          <a:off x="12249150" y="0"/>
+          <a:ext cx="2857501" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -564,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J10" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,14 +576,13 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="80.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -597,9 +593,8 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -610,9 +605,8 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -623,9 +617,8 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -636,9 +629,8 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -649,9 +641,8 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -662,9 +653,8 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -675,9 +665,8 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -688,9 +677,8 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -701,11 +689,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>0</v>
@@ -729,19 +716,16 @@
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="A1:K9"/>
+    <mergeCell ref="A1:J9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">

</xml_diff>

<commit_message>
Fix Female in Excel Template - CAPDEV
</commit_message>
<xml_diff>
--- a/marlo-web/src/main/resources/template/participants-template.xlsx
+++ b/marlo-web/src/main/resources/template/participants-template.xlsx
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,9 +727,12 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J9"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D10 D12:D1048576">
       <formula1>"Male, Famale, Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11">
+      <formula1>"Male, Female, Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>